<commit_message>
grid search + graphs
</commit_message>
<xml_diff>
--- a/papers/Related works results.xlsx
+++ b/papers/Related works results.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TFG\papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952085AE-53E6-494D-8D8C-AF20EF0B4C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4224970-AB06-4A29-A982-E31FF8FA7913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6582" yWindow="6432" windowWidth="23136" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="0" windowWidth="23010" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="related works" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="95">
   <si>
     <t>PAPER</t>
   </si>
@@ -674,12 +685,63 @@
   <si>
     <t>RNN</t>
   </si>
+  <si>
+    <t>paper</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Artificial Neural Network Approach to Football Score Prediction </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(2019)</t>
+    </r>
+  </si>
+  <si>
+    <t>training error</t>
+  </si>
+  <si>
+    <t>train acc</t>
+  </si>
+  <si>
+    <t>test acc</t>
+  </si>
+  <si>
+    <t>MLP 5 units 1 hidden layer with BatchNormalization and 3 output classes</t>
+  </si>
+  <si>
+    <t>architecture</t>
+  </si>
+  <si>
+    <t>optimizer</t>
+  </si>
+  <si>
+    <t>loss</t>
+  </si>
+  <si>
+    <t>CrossEntropy w/o weights</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>SGD
+learn.rate = 1e-1
+batch_size = 20</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -743,6 +805,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -770,7 +862,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -796,22 +888,34 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1096,31 +1200,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="52.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="52.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="8" style="8" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" style="12" customWidth="1"/>
-    <col min="4" max="4" width="51.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="49.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="53.140625" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="23.5546875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="51.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="49.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="7" customWidth="1"/>
+    <col min="7" max="7" width="53.109375" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -1139,14 +1243,14 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:10" ht="192.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="192.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="8">
         <v>2019</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -1162,17 +1266,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="13">
         <v>2014</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="12" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -1181,31 +1285,31 @@
       <c r="F3" s="7">
         <v>85</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="9"/>
+    <row r="4" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="12"/>
       <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="7">
         <v>93</v>
       </c>
-      <c r="G4" s="10"/>
-    </row>
-    <row r="5" spans="1:10" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="1:10" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="13">
         <v>2018</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="10" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1214,40 +1318,40 @@
       <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
+    <row r="6" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
       <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="9"/>
-    </row>
-    <row r="7" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
+      <c r="G6" s="12"/>
+    </row>
+    <row r="7" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
       <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:10" ht="195" x14ac:dyDescent="0.25">
+      <c r="G7" s="12"/>
+    </row>
+    <row r="8" spans="1:10" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="8">
         <v>2020</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="10" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1263,14 +1367,14 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="245.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="245.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="8">
         <v>2021</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="10" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -1286,14 +1390,14 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B10" s="8">
         <v>2015</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="10" t="s">
         <v>36</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -1306,14 +1410,14 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="242.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="262.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B11" s="8">
         <v>2020</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="10" t="s">
         <v>44</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1329,25 +1433,25 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B12" s="8">
         <v>2016</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="189" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B13" s="8">
         <v>2010</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="10" t="s">
         <v>52</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1363,25 +1467,25 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="171" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="171" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B14" s="8">
         <v>2021</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="10" t="s">
         <v>57</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="336" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="336" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="10" t="s">
         <v>60</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1394,33 +1498,33 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="126" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B16" s="8">
         <v>2017</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
       <c r="G16" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="252" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="265.2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B17" s="8">
         <v>2015</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="10" t="s">
         <v>68</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1436,40 +1540,40 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B18" s="8">
         <v>2005</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="14"/>
+      <c r="E18" s="11"/>
       <c r="G18" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B19" s="8">
         <v>2009</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B20" s="8">
         <v>2017</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="10" t="s">
         <v>81</v>
       </c>
       <c r="E20" s="1" t="s">
@@ -1491,4 +1595,78 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC3AC1A7-3FB0-4824-8248-ED1090D3FED6}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.6640625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="30" style="18" customWidth="1"/>
+    <col min="3" max="4" width="15.109375" style="18" customWidth="1"/>
+    <col min="5" max="7" width="12.88671875" style="17" customWidth="1"/>
+    <col min="8" max="8" width="31.109375" style="17" customWidth="1"/>
+    <col min="9" max="16384" width="11.5546875" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="17">
+        <v>1.03</v>
+      </c>
+      <c r="F2" s="17">
+        <v>0.48</v>
+      </c>
+      <c r="G2" s="17">
+        <v>0.11</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update + delete results
</commit_message>
<xml_diff>
--- a/papers/Related works results.xlsx
+++ b/papers/Related works results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TFG\papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0BC087-0EA5-458E-B0D7-1D2808CB89F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A05678-4139-44D3-B40D-E521046E57C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6630" yWindow="6384" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="related works" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="114">
   <si>
     <t>PAPER</t>
   </si>
@@ -796,6 +796,20 @@
   </si>
   <si>
     <t>batch_size = 10</t>
+  </si>
+  <si>
+    <t>~80</t>
+  </si>
+  <si>
+    <t>~80 Combined model
+~60 Grey extreme learning model
+~57 Grey fuzzy model</t>
+  </si>
+  <si>
+    <t>Different predictions in differents moments of the game.</t>
+  </si>
+  <si>
+    <t>63 countries</t>
   </si>
 </sst>
 </file>
@@ -1290,23 +1304,23 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="52.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="52.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.28515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="8" style="8" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" style="10" customWidth="1"/>
-    <col min="4" max="4" width="51.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="49.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" style="7" customWidth="1"/>
-    <col min="7" max="7" width="53.109375" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="1"/>
+    <col min="3" max="3" width="23.5703125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="51.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="49.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="53.140625" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1332,7 +1346,7 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:10" ht="192.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="192.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1355,7 +1369,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>14</v>
       </c>
@@ -1378,7 +1392,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
       <c r="B4" s="25"/>
       <c r="C4" s="26"/>
@@ -1391,7 +1405,7 @@
       </c>
       <c r="G4" s="25"/>
     </row>
-    <row r="5" spans="1:10" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>23</v>
       </c>
@@ -1407,11 +1421,14 @@
       <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="F5" s="7">
+        <v>71.63</v>
+      </c>
       <c r="G5" s="24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
       <c r="B6" s="25"/>
       <c r="D6" s="1" t="s">
@@ -1420,9 +1437,12 @@
       <c r="E6" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="F6" s="7">
+        <v>63.1</v>
+      </c>
       <c r="G6" s="24"/>
     </row>
-    <row r="7" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24"/>
       <c r="B7" s="25"/>
       <c r="D7" s="1" t="s">
@@ -1431,9 +1451,12 @@
       <c r="E7" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="F7" s="7">
+        <v>69.2</v>
+      </c>
       <c r="G7" s="24"/>
     </row>
-    <row r="8" spans="1:10" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="195" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>27</v>
       </c>
@@ -1456,7 +1479,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="245.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="245.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>33</v>
       </c>
@@ -1479,7 +1502,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>35</v>
       </c>
@@ -1499,7 +1522,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="262.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="242.25" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>43</v>
       </c>
@@ -1522,7 +1545,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>45</v>
       </c>
@@ -1533,7 +1556,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="189" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
@@ -1556,7 +1579,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="171" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="171" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>56</v>
       </c>
@@ -1569,8 +1592,14 @@
       <c r="E14" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="336" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="336" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>59</v>
       </c>
@@ -1587,7 +1616,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="126" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>65</v>
       </c>
@@ -1606,7 +1635,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="265.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="267.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>67</v>
       </c>
@@ -1629,7 +1658,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>72</v>
       </c>
@@ -1644,7 +1673,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>75</v>
       </c>
@@ -1655,7 +1684,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>80</v>
       </c>
@@ -1665,8 +1694,14 @@
       <c r="C20" s="10" t="s">
         <v>81</v>
       </c>
+      <c r="D20" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="E20" s="1" t="s">
         <v>82</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1694,20 +1729,20 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.6640625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" style="13" customWidth="1"/>
     <col min="2" max="2" width="30" style="14" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" style="14" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" style="14" customWidth="1"/>
-    <col min="5" max="5" width="19.44140625" style="22" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" style="14" customWidth="1"/>
-    <col min="7" max="9" width="9.44140625" style="13" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" style="13" customWidth="1"/>
-    <col min="11" max="16384" width="11.5546875" style="13"/>
+    <col min="3" max="3" width="13.85546875" style="14" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="14" customWidth="1"/>
+    <col min="7" max="9" width="9.42578125" style="13" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" style="13" customWidth="1"/>
+    <col min="11" max="16384" width="11.5703125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>83</v>
       </c>
@@ -1745,7 +1780,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>84</v>
       </c>
@@ -1774,7 +1809,7 @@
         <v>0.59499999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="36" x14ac:dyDescent="0.25">
       <c r="C3" s="14" t="s">
         <v>98</v>
       </c>
@@ -1797,7 +1832,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="36" x14ac:dyDescent="0.25">
       <c r="C4" s="14" t="s">
         <v>93</v>
       </c>
@@ -1820,7 +1855,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="36" x14ac:dyDescent="0.25">
       <c r="C5" s="14" t="s">
         <v>107</v>
       </c>
@@ -1852,7 +1887,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="48" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="48" x14ac:dyDescent="0.25">
       <c r="C6" s="14" t="s">
         <v>109</v>
       </c>
@@ -1899,18 +1934,18 @@
       <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="21"/>
-    <col min="5" max="5" width="5.5546875" style="16" customWidth="1"/>
-    <col min="6" max="6" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" style="21"/>
+    <col min="5" max="5" width="5.5703125" style="16" customWidth="1"/>
+    <col min="6" max="6" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" style="18"/>
-    <col min="9" max="9" width="11.5546875" style="21"/>
-    <col min="13" max="13" width="11.5546875" style="16"/>
+    <col min="8" max="8" width="11.5703125" style="18"/>
+    <col min="9" max="9" width="11.5703125" style="21"/>
+    <col min="13" max="13" width="11.5703125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="28"/>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -1924,371 +1959,371 @@
       <c r="M1" s="28"/>
       <c r="N1" s="28"/>
     </row>
-    <row r="2" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>
       <c r="E2" s="20"/>
       <c r="H2" s="18"/>
       <c r="I2" s="19"/>
       <c r="M2" s="20"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H3" s="27"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H4" s="27"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H5" s="27"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H6" s="27"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H7" s="27"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H8" s="27"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H9" s="27"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H10" s="27"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H11" s="27"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H12" s="27"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H13" s="27"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H14" s="27"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H15" s="27"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H16" s="27"/>
     </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H17" s="27"/>
     </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H18" s="27"/>
     </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H19" s="27"/>
     </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H20" s="27"/>
     </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H21" s="27"/>
     </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H22" s="27"/>
     </row>
-    <row r="23" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H23" s="27"/>
     </row>
-    <row r="24" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H24" s="27"/>
     </row>
-    <row r="25" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H25" s="27"/>
     </row>
-    <row r="26" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H26" s="27"/>
     </row>
-    <row r="27" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H27" s="27"/>
     </row>
-    <row r="28" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H28" s="27"/>
     </row>
-    <row r="29" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H29" s="27"/>
     </row>
-    <row r="30" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H30" s="27"/>
     </row>
-    <row r="31" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H31" s="27"/>
     </row>
-    <row r="32" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H32" s="27"/>
     </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H33" s="27"/>
     </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H34" s="27"/>
     </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H35" s="27"/>
     </row>
-    <row r="36" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H36" s="27"/>
     </row>
-    <row r="37" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H37" s="27"/>
     </row>
-    <row r="38" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H38" s="27"/>
     </row>
-    <row r="39" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H39" s="27"/>
     </row>
-    <row r="40" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H40" s="27"/>
     </row>
-    <row r="41" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H41" s="27"/>
     </row>
-    <row r="42" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H42" s="27"/>
     </row>
-    <row r="43" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H43" s="17"/>
     </row>
-    <row r="44" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H44" s="27"/>
     </row>
-    <row r="45" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H45" s="27"/>
     </row>
-    <row r="46" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H46" s="27"/>
     </row>
-    <row r="47" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H47" s="27"/>
     </row>
-    <row r="48" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H48" s="27"/>
     </row>
-    <row r="49" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H49" s="27"/>
     </row>
-    <row r="50" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H50" s="27"/>
     </row>
-    <row r="51" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H51" s="27"/>
     </row>
-    <row r="52" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H52" s="27"/>
     </row>
-    <row r="53" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H53" s="27"/>
     </row>
-    <row r="54" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H54" s="27"/>
     </row>
-    <row r="55" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H55" s="27"/>
     </row>
-    <row r="56" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H56" s="27"/>
     </row>
-    <row r="57" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H57" s="27"/>
     </row>
-    <row r="58" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H58" s="27"/>
     </row>
-    <row r="59" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H59" s="27"/>
     </row>
-    <row r="60" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H60" s="27"/>
     </row>
-    <row r="61" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H61" s="27"/>
     </row>
-    <row r="62" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H62" s="27"/>
     </row>
-    <row r="63" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H63" s="27"/>
     </row>
-    <row r="64" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H64" s="27"/>
     </row>
-    <row r="65" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H65" s="27"/>
     </row>
-    <row r="66" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H66" s="27"/>
     </row>
-    <row r="67" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H67" s="27"/>
     </row>
-    <row r="68" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H68" s="27"/>
     </row>
-    <row r="69" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H69" s="27"/>
     </row>
-    <row r="70" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H70" s="27"/>
     </row>
-    <row r="71" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H71" s="27"/>
     </row>
-    <row r="72" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H72" s="27"/>
     </row>
-    <row r="73" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H73" s="27"/>
     </row>
-    <row r="74" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H74" s="27"/>
     </row>
-    <row r="75" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H75" s="27"/>
     </row>
-    <row r="76" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H76" s="27"/>
     </row>
-    <row r="77" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H77" s="27"/>
     </row>
-    <row r="78" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H78" s="27"/>
     </row>
-    <row r="79" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H79" s="27"/>
     </row>
-    <row r="80" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H80" s="27"/>
     </row>
-    <row r="81" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H81" s="27"/>
     </row>
-    <row r="82" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H82" s="27"/>
     </row>
-    <row r="83" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H83" s="27"/>
     </row>
-    <row r="85" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H85" s="27"/>
     </row>
-    <row r="86" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H86" s="27"/>
     </row>
-    <row r="87" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H87" s="27"/>
     </row>
-    <row r="88" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H88" s="27"/>
     </row>
-    <row r="89" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H89" s="27"/>
     </row>
-    <row r="90" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H90" s="27"/>
     </row>
-    <row r="91" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H91" s="27"/>
     </row>
-    <row r="92" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H92" s="27"/>
     </row>
-    <row r="93" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H93" s="27"/>
     </row>
-    <row r="94" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H94" s="27"/>
     </row>
-    <row r="95" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H95" s="27"/>
     </row>
-    <row r="96" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H96" s="27"/>
     </row>
-    <row r="97" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H97" s="27"/>
     </row>
-    <row r="98" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H98" s="27"/>
     </row>
-    <row r="99" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H99" s="27"/>
     </row>
-    <row r="100" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H100" s="27"/>
     </row>
-    <row r="101" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H101" s="27"/>
     </row>
-    <row r="102" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H102" s="27"/>
     </row>
-    <row r="103" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H103" s="27"/>
     </row>
-    <row r="104" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H104" s="27"/>
     </row>
-    <row r="105" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H105" s="27"/>
     </row>
-    <row r="106" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H106" s="27"/>
     </row>
-    <row r="107" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H107" s="27"/>
     </row>
-    <row r="108" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H108" s="27"/>
     </row>
-    <row r="109" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H109" s="27"/>
     </row>
-    <row r="110" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H110" s="27"/>
     </row>
-    <row r="111" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H111" s="27"/>
     </row>
-    <row r="112" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H112" s="27"/>
     </row>
-    <row r="113" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H113" s="27"/>
     </row>
-    <row r="114" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H114" s="27"/>
     </row>
-    <row r="115" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H115" s="27"/>
     </row>
-    <row r="116" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H116" s="27"/>
     </row>
-    <row r="117" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H117" s="27"/>
     </row>
-    <row r="118" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H118" s="27"/>
     </row>
-    <row r="119" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H119" s="27"/>
     </row>
-    <row r="120" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H120" s="27"/>
     </row>
-    <row r="121" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H121" s="27"/>
     </row>
-    <row r="122" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H122" s="27"/>
     </row>
-    <row r="123" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H123" s="27"/>
     </row>
   </sheetData>

</xml_diff>